<commit_message>
fixing db and columns
</commit_message>
<xml_diff>
--- a/Engine/db/db.xlsx
+++ b/Engine/db/db.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hamza\github\Rapport-Journalier\Engine\db\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\Github\generetor\Engine\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD05E35-C863-4EE3-8AB1-6BB32263C2ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E531FF-A022-42C3-AF78-22CA3CB6DC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TypeProducts" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'% FACTURATION'!$B$1:$C$52</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DB!$A$1:$W$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DB!$A$1:$W$53</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">DB!$A$1:$X$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1203,15 +1203,15 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1222,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1262,7 +1262,7 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1280,7 +1280,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1288,7 +1288,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -1296,23 +1296,23 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
     </row>
   </sheetData>
@@ -1328,38 +1328,38 @@
   </sheetPr>
   <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView zoomScale="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J38" sqref="J38"/>
-      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" style="1" customWidth="1"/>
-    <col min="3" max="4" width="19.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" style="1" customWidth="1"/>
+    <col min="3" max="4" width="19.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="17.88671875" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
     <col min="10" max="10" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.33203125" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
     <col min="13" max="13" width="28" customWidth="1"/>
-    <col min="14" max="14" width="18.42578125" customWidth="1"/>
-    <col min="15" max="15" width="27.5703125" customWidth="1"/>
-    <col min="16" max="16" width="27.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="34.42578125" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" customWidth="1"/>
-    <col min="19" max="19" width="26.42578125" customWidth="1"/>
-    <col min="20" max="20" width="23.85546875" customWidth="1"/>
-    <col min="21" max="22" width="24.140625" customWidth="1"/>
-    <col min="23" max="23" width="22.7109375" customWidth="1"/>
+    <col min="14" max="14" width="18.44140625" customWidth="1"/>
+    <col min="15" max="15" width="27.5546875" customWidth="1"/>
+    <col min="16" max="16" width="27.5546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="34.44140625" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" customWidth="1"/>
+    <col min="19" max="19" width="26.44140625" customWidth="1"/>
+    <col min="20" max="20" width="23.88671875" customWidth="1"/>
+    <col min="21" max="22" width="24.109375" customWidth="1"/>
+    <col min="23" max="23" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>28</v>
       </c>
@@ -1501,7 +1501,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>31</v>
       </c>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>33</v>
       </c>
@@ -1643,7 +1643,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>35</v>
       </c>
@@ -1651,16 +1651,16 @@
         <v>36</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D5" s="13">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="E5" s="14">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="F5" s="14">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="G5" s="14">
         <v>0</v>
@@ -1669,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="14">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="J5" s="14">
         <v>0</v>
@@ -1678,7 +1678,7 @@
         <v>0</v>
       </c>
       <c r="L5" s="14">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="M5" s="14">
         <v>0</v>
@@ -1687,19 +1687,19 @@
         <v>0</v>
       </c>
       <c r="O5" s="14">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="P5" s="14">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="Q5" s="14">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="R5" s="14">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="S5" s="14">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="T5" s="14">
         <v>0</v>
@@ -1711,10 +1711,10 @@
         <v>0</v>
       </c>
       <c r="W5" s="14">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>37</v>
       </c>
@@ -1785,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>39</v>
       </c>
@@ -1856,7 +1856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>41</v>
       </c>
@@ -1927,7 +1927,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>43</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>45</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>47</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>49</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>51</v>
       </c>
@@ -2282,7 +2282,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>53</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>55</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>57</v>
       </c>
@@ -2495,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>60</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>62</v>
       </c>
@@ -2625,19 +2625,19 @@
         <v>0</v>
       </c>
       <c r="T18" s="14">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="U18" s="14">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="V18" s="14">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="W18" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>64</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>66</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>68</v>
       </c>
@@ -2850,7 +2850,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>70</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>72</v>
       </c>
@@ -2992,7 +2992,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>74</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:23" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>76</v>
       </c>
@@ -3071,13 +3071,13 @@
         <v>77</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="D25" s="14">
         <v>50</v>
       </c>
       <c r="E25" s="14">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F25" s="14">
         <v>0</v>
@@ -3134,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>78</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>80</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>82</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>84</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>86</v>
       </c>
@@ -3489,7 +3489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>88</v>
       </c>
@@ -3560,7 +3560,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>90</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>92</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>94</v>
       </c>
@@ -3773,7 +3773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>96</v>
       </c>
@@ -3844,7 +3844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>98</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>100</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>102</v>
       </c>
@@ -4057,7 +4057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>104</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>106</v>
       </c>
@@ -4199,7 +4199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>108</v>
       </c>
@@ -4270,7 +4270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>110</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>112</v>
       </c>
@@ -4412,7 +4412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>114</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>116</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>118</v>
       </c>
@@ -4625,7 +4625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>119</v>
       </c>
@@ -4696,7 +4696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>121</v>
       </c>
@@ -4767,7 +4767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>123</v>
       </c>
@@ -4838,7 +4838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>125</v>
       </c>
@@ -4909,7 +4909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>127</v>
       </c>
@@ -4980,7 +4980,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>163</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>165</v>
       </c>
@@ -5134,17 +5134,17 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="1"/>
+    <col min="2" max="2" width="11.44140625" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="17" t="s">
         <v>129</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="19" t="s">
         <v>131</v>
       </c>
@@ -5160,7 +5160,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>132</v>
       </c>
@@ -5168,7 +5168,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
         <v>133</v>
       </c>
@@ -5176,7 +5176,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>133</v>
       </c>
@@ -5184,7 +5184,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="21" t="s">
         <v>133</v>
       </c>
@@ -5192,7 +5192,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="21" t="s">
         <v>133</v>
       </c>
@@ -5200,7 +5200,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="23" t="s">
         <v>133</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="21" t="s">
         <v>135</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
         <v>135</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="21" t="s">
         <v>136</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="21" t="s">
         <v>162</v>
       </c>
@@ -5240,7 +5240,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="21" t="s">
         <v>162</v>
       </c>
@@ -5248,7 +5248,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
         <v>138</v>
       </c>
@@ -5256,7 +5256,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
         <v>139</v>
       </c>
@@ -5264,7 +5264,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="23" t="s">
         <v>140</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="23" t="s">
         <v>141</v>
       </c>
@@ -5280,7 +5280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="23" t="s">
         <v>141</v>
       </c>
@@ -5288,7 +5288,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="25" t="s">
         <v>142</v>
       </c>
@@ -5310,17 +5310,17 @@
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1"/>
-    <col min="4" max="4" width="28.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1"/>
+    <col min="1" max="1" width="5.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.88671875" bestFit="1"/>
+    <col min="4" max="4" width="28.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.109375" bestFit="1"/>
     <col min="6" max="6" width="21" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="27" t="s">
         <v>143</v>
       </c>
@@ -5337,7 +5337,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="29" t="s">
         <v>148</v>
@@ -5355,7 +5355,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="29" t="s">
         <v>148</v>
       </c>
@@ -5372,7 +5372,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="33" t="s">
         <v>152</v>
       </c>
@@ -5389,7 +5389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="33" t="s">
         <v>152</v>
       </c>
@@ -5404,7 +5404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="34" t="s">
         <v>155</v>
       </c>
@@ -5421,7 +5421,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="37"/>
       <c r="B7" s="38" t="s">
         <v>157</v>
@@ -5439,7 +5439,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="42"/>
       <c r="B8" s="38" t="s">
         <v>164</v>
@@ -5455,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="41" t="s">
         <v>148</v>
       </c>
@@ -5482,17 +5482,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="34.5703125" bestFit="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1"/>
+    <col min="2" max="2" width="34.5546875" bestFit="1"/>
+    <col min="3" max="3" width="10.44140625" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="48" t="s">
         <v>23</v>
       </c>
@@ -5500,7 +5500,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B2" s="44" t="s">
         <v>29</v>
       </c>
@@ -5508,7 +5508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B3" s="45" t="s">
         <v>32</v>
       </c>
@@ -5516,7 +5516,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B4" s="45" t="s">
         <v>34</v>
       </c>
@@ -5525,7 +5525,7 @@
       </c>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B5" s="45" t="s">
         <v>36</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B6" s="45" t="s">
         <v>38</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B7" s="45" t="s">
         <v>124</v>
       </c>
@@ -5549,7 +5549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B8" s="45" t="s">
         <v>42</v>
       </c>
@@ -5557,7 +5557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B9" s="46" t="s">
         <v>44</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B10" s="46" t="s">
         <v>46</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B11" s="46" t="s">
         <v>48</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B12" s="46" t="s">
         <v>50</v>
       </c>
@@ -5589,7 +5589,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B13" s="46" t="s">
         <v>52</v>
       </c>
@@ -5597,7 +5597,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B14" s="46" t="s">
         <v>54</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B15" s="46" t="s">
         <v>56</v>
       </c>
@@ -5613,7 +5613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B16" s="46" t="s">
         <v>58</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B17" s="46" t="s">
         <v>61</v>
       </c>
@@ -5629,7 +5629,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B18" s="46" t="s">
         <v>63</v>
       </c>
@@ -5637,7 +5637,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B19" s="46" t="s">
         <v>65</v>
       </c>
@@ -5645,7 +5645,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B20" s="46" t="s">
         <v>67</v>
       </c>
@@ -5653,7 +5653,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="21" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B21" s="46" t="s">
         <v>69</v>
       </c>
@@ -5661,7 +5661,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="46" t="s">
         <v>71</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B23" s="46" t="s">
         <v>73</v>
       </c>
@@ -5677,7 +5677,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B24" s="46" t="s">
         <v>75</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B25" s="46" t="s">
         <v>77</v>
       </c>
@@ -5693,7 +5693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="46" t="s">
         <v>79</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B27" s="46" t="s">
         <v>81</v>
       </c>
@@ -5709,7 +5709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B28" s="46" t="s">
         <v>83</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B29" s="46" t="s">
         <v>85</v>
       </c>
@@ -5725,7 +5725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" s="46" t="s">
         <v>87</v>
       </c>
@@ -5733,7 +5733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B31" s="46" t="s">
         <v>126</v>
       </c>
@@ -5741,7 +5741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="46" t="s">
         <v>89</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B33" s="46" t="s">
         <v>91</v>
       </c>
@@ -5757,7 +5757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B34" s="46" t="s">
         <v>93</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B35" s="46" t="s">
         <v>95</v>
       </c>
@@ -5773,7 +5773,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="36" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B36" s="46" t="s">
         <v>97</v>
       </c>
@@ -5781,7 +5781,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B37" s="46" t="s">
         <v>99</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B38" s="46" t="s">
         <v>101</v>
       </c>
@@ -5797,7 +5797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B39" s="46" t="s">
         <v>103</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B40" s="46" t="s">
         <v>105</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B41" s="46" t="s">
         <v>107</v>
       </c>
@@ -5821,7 +5821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B42" s="46" t="s">
         <v>109</v>
       </c>
@@ -5829,7 +5829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B43" s="46" t="s">
         <v>111</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B44" s="46" t="s">
         <v>113</v>
       </c>
@@ -5845,7 +5845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B45" s="46" t="s">
         <v>115</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B46" s="46" t="s">
         <v>117</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B47" s="46" t="s">
         <v>40</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B48" s="46" t="s">
         <v>120</v>
       </c>
@@ -5877,7 +5877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="2:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B49" s="46" t="s">
         <v>122</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B50" s="45" t="s">
         <v>128</v>
       </c>
@@ -5893,7 +5893,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="2:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:3" ht="15.6" x14ac:dyDescent="0.25">
       <c r="B51" s="45" t="s">
         <v>164</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" ht="16.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="47" t="s">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
adding more to the db .
</commit_message>
<xml_diff>
--- a/Engine/db/db.xlsx
+++ b/Engine/db/db.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\Github\generetor\Engine\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E531FF-A022-42C3-AF78-22CA3CB6DC3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3598EFD-685F-471B-80FD-8EBFDBA2324E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,8 +21,8 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'% FACTURATION'!$B$1:$C$52</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DB!$A$1:$W$53</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">DB!$A$1:$X$30</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DB!$A$1:$X$53</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">DB!$A$1:$Y$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="168">
   <si>
     <t>GRAVES</t>
   </si>
@@ -541,6 +541,9 @@
   </si>
   <si>
     <t>KASAL TRAVEAUX</t>
+  </si>
+  <si>
+    <t>GRAVETTE G1 10/20</t>
   </si>
 </sst>
 </file>
@@ -1197,10 +1200,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1211,7 +1214,7 @@
     <col min="4" max="4" width="17.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1233,7 +1236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1244,7 +1247,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1253,7 +1256,7 @@
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
@@ -1262,58 +1265,70 @@
       </c>
       <c r="D5" s="1"/>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="C11" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="3" t="s">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="3" t="s">
+    <row r="13" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13"/>
+      <c r="C13" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="1"/>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1326,12 +1341,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W53"/>
+  <dimension ref="A1:X53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J38" sqref="J38"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="L54" sqref="L54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1346,20 +1361,21 @@
     <col min="9" max="9" width="20.33203125" customWidth="1"/>
     <col min="10" max="10" width="22" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.33203125" customWidth="1"/>
-    <col min="12" max="12" width="20" customWidth="1"/>
-    <col min="13" max="13" width="28" customWidth="1"/>
-    <col min="14" max="14" width="18.44140625" customWidth="1"/>
-    <col min="15" max="15" width="27.5546875" customWidth="1"/>
-    <col min="16" max="16" width="27.5546875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="34.44140625" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" customWidth="1"/>
-    <col min="19" max="19" width="26.44140625" customWidth="1"/>
-    <col min="20" max="20" width="23.88671875" customWidth="1"/>
-    <col min="21" max="22" width="24.109375" customWidth="1"/>
-    <col min="23" max="23" width="22.6640625" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="14" max="14" width="28" customWidth="1"/>
+    <col min="15" max="15" width="18.44140625" customWidth="1"/>
+    <col min="16" max="16" width="27.5546875" customWidth="1"/>
+    <col min="17" max="17" width="27.5546875" style="1" customWidth="1"/>
+    <col min="18" max="18" width="34.44140625" customWidth="1"/>
+    <col min="19" max="19" width="13.88671875" customWidth="1"/>
+    <col min="20" max="20" width="26.44140625" customWidth="1"/>
+    <col min="21" max="21" width="23.88671875" customWidth="1"/>
+    <col min="22" max="23" width="24.109375" customWidth="1"/>
+    <col min="24" max="24" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>22</v>
       </c>
@@ -1394,43 +1410,46 @@
         <v>13</v>
       </c>
       <c r="L1" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="N1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="7" t="s">
+      <c r="U1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="X1" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>28</v>
       </c>
@@ -1465,7 +1484,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="14">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="M2" s="14">
         <v>75</v>
@@ -1474,20 +1493,20 @@
         <v>75</v>
       </c>
       <c r="O2" s="14">
+        <v>75</v>
+      </c>
+      <c r="P2" s="14">
         <v>70</v>
       </c>
-      <c r="P2" s="14">
-        <v>0</v>
-      </c>
       <c r="Q2" s="14">
         <v>0</v>
       </c>
       <c r="R2" s="14">
+        <v>0</v>
+      </c>
+      <c r="S2" s="14">
         <v>25</v>
       </c>
-      <c r="S2" s="14">
-        <v>0</v>
-      </c>
       <c r="T2" s="14">
         <v>0</v>
       </c>
@@ -1498,10 +1517,13 @@
         <v>0</v>
       </c>
       <c r="W2" s="14">
+        <v>0</v>
+      </c>
+      <c r="X2" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>31</v>
       </c>
@@ -1536,43 +1558,46 @@
         <v>0</v>
       </c>
       <c r="L3" s="14">
+        <v>0</v>
+      </c>
+      <c r="M3" s="14">
         <v>74</v>
       </c>
-      <c r="M3" s="14">
-        <v>0</v>
-      </c>
       <c r="N3" s="14">
         <v>0</v>
       </c>
       <c r="O3" s="14">
+        <v>0</v>
+      </c>
+      <c r="P3" s="14">
         <v>70</v>
       </c>
-      <c r="P3" s="14">
-        <v>0</v>
-      </c>
       <c r="Q3" s="14">
+        <v>0</v>
+      </c>
+      <c r="R3" s="14">
         <v>61</v>
       </c>
-      <c r="R3" s="14">
+      <c r="S3" s="14">
         <v>25</v>
       </c>
-      <c r="S3" s="14">
+      <c r="T3" s="14">
         <v>16</v>
       </c>
-      <c r="T3" s="14">
-        <v>0</v>
-      </c>
       <c r="U3" s="14">
+        <v>0</v>
+      </c>
+      <c r="V3" s="14">
         <v>56</v>
       </c>
-      <c r="V3" s="14">
+      <c r="W3" s="14">
         <v>55</v>
       </c>
-      <c r="W3" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X3" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>33</v>
       </c>
@@ -1607,29 +1632,29 @@
         <v>0</v>
       </c>
       <c r="L4" s="14">
+        <v>0</v>
+      </c>
+      <c r="M4" s="14">
         <v>75</v>
       </c>
-      <c r="M4" s="14">
-        <v>0</v>
-      </c>
       <c r="N4" s="14">
         <v>0</v>
       </c>
       <c r="O4" s="14">
+        <v>0</v>
+      </c>
+      <c r="P4" s="14">
         <v>70</v>
       </c>
-      <c r="P4" s="14">
-        <v>0</v>
-      </c>
       <c r="Q4" s="14">
         <v>0</v>
       </c>
       <c r="R4" s="14">
+        <v>0</v>
+      </c>
+      <c r="S4" s="14">
         <v>25</v>
       </c>
-      <c r="S4" s="14">
-        <v>0</v>
-      </c>
       <c r="T4" s="14">
         <v>0</v>
       </c>
@@ -1640,10 +1665,13 @@
         <v>0</v>
       </c>
       <c r="W4" s="14">
+        <v>0</v>
+      </c>
+      <c r="X4" s="14">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>35</v>
       </c>
@@ -1678,16 +1706,16 @@
         <v>0</v>
       </c>
       <c r="L5" s="14">
+        <v>0</v>
+      </c>
+      <c r="M5" s="14">
         <v>50</v>
       </c>
-      <c r="M5" s="14">
-        <v>0</v>
-      </c>
       <c r="N5" s="14">
         <v>0</v>
       </c>
       <c r="O5" s="14">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="P5" s="14">
         <v>48</v>
@@ -1696,13 +1724,13 @@
         <v>48</v>
       </c>
       <c r="R5" s="14">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="S5" s="14">
         <v>15</v>
       </c>
       <c r="T5" s="14">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="U5" s="14">
         <v>0</v>
@@ -1711,10 +1739,13 @@
         <v>0</v>
       </c>
       <c r="W5" s="14">
+        <v>0</v>
+      </c>
+      <c r="X5" s="14">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>37</v>
       </c>
@@ -1758,34 +1789,37 @@
         <v>0</v>
       </c>
       <c r="O6" s="14">
+        <v>0</v>
+      </c>
+      <c r="P6" s="14">
         <v>75</v>
       </c>
-      <c r="P6" s="14">
-        <v>0</v>
-      </c>
       <c r="Q6" s="14">
         <v>0</v>
       </c>
       <c r="R6" s="14">
+        <v>0</v>
+      </c>
+      <c r="S6" s="14">
         <v>25</v>
       </c>
-      <c r="S6" s="14">
-        <v>0</v>
-      </c>
       <c r="T6" s="14">
+        <v>0</v>
+      </c>
+      <c r="U6" s="14">
         <v>58</v>
       </c>
-      <c r="U6" s="14">
+      <c r="V6" s="14">
         <v>62</v>
       </c>
-      <c r="V6" s="14">
-        <v>0</v>
-      </c>
       <c r="W6" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X6" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>39</v>
       </c>
@@ -1855,8 +1889,11 @@
       <c r="W7" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X7" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>41</v>
       </c>
@@ -1891,20 +1928,20 @@
         <v>0</v>
       </c>
       <c r="L8" s="14">
+        <v>0</v>
+      </c>
+      <c r="M8" s="14">
         <v>75</v>
       </c>
-      <c r="M8" s="14">
-        <v>0</v>
-      </c>
       <c r="N8" s="14">
+        <v>0</v>
+      </c>
+      <c r="O8" s="14">
         <v>41</v>
       </c>
-      <c r="O8" s="14">
+      <c r="P8" s="14">
         <v>75</v>
       </c>
-      <c r="P8" s="14">
-        <v>0</v>
-      </c>
       <c r="Q8" s="14">
         <v>0</v>
       </c>
@@ -1915,7 +1952,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="14">
-        <v>56</v>
+        <v>0</v>
       </c>
       <c r="U8" s="14">
         <v>56</v>
@@ -1926,8 +1963,11 @@
       <c r="W8" s="14">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X8" s="14">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>43</v>
       </c>
@@ -1962,29 +2002,29 @@
         <v>0</v>
       </c>
       <c r="L9" s="14">
+        <v>0</v>
+      </c>
+      <c r="M9" s="14">
         <v>75</v>
       </c>
-      <c r="M9" s="14">
-        <v>0</v>
-      </c>
       <c r="N9" s="14">
         <v>0</v>
       </c>
       <c r="O9" s="14">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="P9" s="14">
         <v>75</v>
       </c>
       <c r="Q9" s="14">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="R9" s="14">
+        <v>0</v>
+      </c>
+      <c r="S9" s="14">
         <v>25</v>
       </c>
-      <c r="S9" s="14">
-        <v>0</v>
-      </c>
       <c r="T9" s="14">
         <v>0</v>
       </c>
@@ -1995,10 +2035,13 @@
         <v>0</v>
       </c>
       <c r="W9" s="14">
+        <v>0</v>
+      </c>
+      <c r="X9" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>45</v>
       </c>
@@ -2033,29 +2076,29 @@
         <v>0</v>
       </c>
       <c r="L10" s="14">
+        <v>0</v>
+      </c>
+      <c r="M10" s="14">
         <v>70</v>
       </c>
-      <c r="M10" s="14">
-        <v>0</v>
-      </c>
       <c r="N10" s="14">
         <v>0</v>
       </c>
       <c r="O10" s="14">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="P10" s="14">
         <v>70</v>
       </c>
       <c r="Q10" s="14">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="R10" s="14">
+        <v>0</v>
+      </c>
+      <c r="S10" s="14">
         <v>25</v>
       </c>
-      <c r="S10" s="14">
-        <v>0</v>
-      </c>
       <c r="T10" s="14">
         <v>0</v>
       </c>
@@ -2066,10 +2109,13 @@
         <v>0</v>
       </c>
       <c r="W10" s="14">
+        <v>0</v>
+      </c>
+      <c r="X10" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>47</v>
       </c>
@@ -2104,29 +2150,29 @@
         <v>0</v>
       </c>
       <c r="L11" s="14">
+        <v>0</v>
+      </c>
+      <c r="M11" s="14">
         <v>75</v>
       </c>
-      <c r="M11" s="14">
-        <v>0</v>
-      </c>
       <c r="N11" s="14">
         <v>0</v>
       </c>
       <c r="O11" s="14">
+        <v>0</v>
+      </c>
+      <c r="P11" s="14">
         <v>75</v>
       </c>
-      <c r="P11" s="14">
-        <v>0</v>
-      </c>
       <c r="Q11" s="14">
         <v>0</v>
       </c>
       <c r="R11" s="14">
+        <v>0</v>
+      </c>
+      <c r="S11" s="14">
         <v>23</v>
       </c>
-      <c r="S11" s="14">
-        <v>0</v>
-      </c>
       <c r="T11" s="14">
         <v>0</v>
       </c>
@@ -2137,10 +2183,13 @@
         <v>0</v>
       </c>
       <c r="W11" s="14">
+        <v>0</v>
+      </c>
+      <c r="X11" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>49</v>
       </c>
@@ -2175,29 +2224,29 @@
         <v>0</v>
       </c>
       <c r="L12" s="14">
+        <v>0</v>
+      </c>
+      <c r="M12" s="14">
         <v>68</v>
       </c>
-      <c r="M12" s="14">
-        <v>0</v>
-      </c>
       <c r="N12" s="14">
         <v>0</v>
       </c>
       <c r="O12" s="14">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="P12" s="14">
         <v>68</v>
       </c>
       <c r="Q12" s="14">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="R12" s="14">
+        <v>0</v>
+      </c>
+      <c r="S12" s="14">
         <v>25</v>
       </c>
-      <c r="S12" s="14">
-        <v>0</v>
-      </c>
       <c r="T12" s="14">
         <v>0</v>
       </c>
@@ -2208,10 +2257,13 @@
         <v>0</v>
       </c>
       <c r="W12" s="14">
+        <v>0</v>
+      </c>
+      <c r="X12" s="14">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>51</v>
       </c>
@@ -2246,34 +2298,34 @@
         <v>0</v>
       </c>
       <c r="L13" s="14">
+        <v>0</v>
+      </c>
+      <c r="M13" s="14">
         <v>75</v>
       </c>
-      <c r="M13" s="14">
-        <v>0</v>
-      </c>
       <c r="N13" s="14">
+        <v>0</v>
+      </c>
+      <c r="O13" s="14">
         <v>48</v>
-      </c>
-      <c r="O13" s="14">
-        <v>72</v>
       </c>
       <c r="P13" s="14">
         <v>72</v>
       </c>
       <c r="Q13" s="14">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="R13" s="14">
+        <v>0</v>
+      </c>
+      <c r="S13" s="14">
         <v>25</v>
       </c>
-      <c r="S13" s="14">
-        <v>0</v>
-      </c>
       <c r="T13" s="14">
+        <v>0</v>
+      </c>
+      <c r="U13" s="14">
         <v>48</v>
-      </c>
-      <c r="U13" s="14">
-        <v>57</v>
       </c>
       <c r="V13" s="14">
         <v>57</v>
@@ -2281,8 +2333,11 @@
       <c r="W13" s="14">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X13" s="14">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>53</v>
       </c>
@@ -2317,23 +2372,23 @@
         <v>0</v>
       </c>
       <c r="L14" s="14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="14">
         <v>75</v>
       </c>
-      <c r="M14" s="14">
-        <v>0</v>
-      </c>
       <c r="N14" s="14">
         <v>0</v>
       </c>
       <c r="O14" s="14">
+        <v>0</v>
+      </c>
+      <c r="P14" s="14">
         <v>70</v>
       </c>
-      <c r="P14" s="14">
+      <c r="Q14" s="14">
         <v>75</v>
       </c>
-      <c r="Q14" s="14">
-        <v>0</v>
-      </c>
       <c r="R14" s="14">
         <v>0</v>
       </c>
@@ -2352,8 +2407,11 @@
       <c r="W14" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X14" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>55</v>
       </c>
@@ -2388,20 +2446,20 @@
         <v>0</v>
       </c>
       <c r="L15" s="14">
+        <v>0</v>
+      </c>
+      <c r="M15" s="14">
         <v>112</v>
       </c>
-      <c r="M15" s="14">
-        <v>0</v>
-      </c>
       <c r="N15" s="14">
         <v>0</v>
       </c>
       <c r="O15" s="14">
+        <v>0</v>
+      </c>
+      <c r="P15" s="14">
         <v>110</v>
       </c>
-      <c r="P15" s="14">
-        <v>0</v>
-      </c>
       <c r="Q15" s="14">
         <v>0</v>
       </c>
@@ -2423,8 +2481,11 @@
       <c r="W15" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>57</v>
       </c>
@@ -2459,20 +2520,20 @@
         <v>0</v>
       </c>
       <c r="L16" s="14">
+        <v>0</v>
+      </c>
+      <c r="M16" s="14">
         <v>50</v>
       </c>
-      <c r="M16" s="14">
-        <v>0</v>
-      </c>
       <c r="N16" s="14">
         <v>0</v>
       </c>
       <c r="O16" s="14">
+        <v>0</v>
+      </c>
+      <c r="P16" s="14">
         <v>45</v>
       </c>
-      <c r="P16" s="14">
-        <v>0</v>
-      </c>
       <c r="Q16" s="14">
         <v>0</v>
       </c>
@@ -2494,8 +2555,11 @@
       <c r="W16" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X16" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>60</v>
       </c>
@@ -2530,29 +2594,29 @@
         <v>0</v>
       </c>
       <c r="L17" s="14">
+        <v>0</v>
+      </c>
+      <c r="M17" s="14">
         <v>70</v>
       </c>
-      <c r="M17" s="14">
-        <v>0</v>
-      </c>
       <c r="N17" s="14">
         <v>0</v>
       </c>
       <c r="O17" s="14">
+        <v>0</v>
+      </c>
+      <c r="P17" s="14">
         <v>70</v>
       </c>
-      <c r="P17" s="14">
-        <v>0</v>
-      </c>
       <c r="Q17" s="14">
         <v>0</v>
       </c>
       <c r="R17" s="14">
+        <v>0</v>
+      </c>
+      <c r="S17" s="14">
         <v>25</v>
       </c>
-      <c r="S17" s="14">
-        <v>0</v>
-      </c>
       <c r="T17" s="14">
         <v>0</v>
       </c>
@@ -2563,10 +2627,13 @@
         <v>0</v>
       </c>
       <c r="W17" s="14">
+        <v>0</v>
+      </c>
+      <c r="X17" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>62</v>
       </c>
@@ -2586,10 +2653,10 @@
         <v>60</v>
       </c>
       <c r="G18" s="14">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="H18" s="14">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="I18" s="14">
         <v>68</v>
@@ -2604,28 +2671,28 @@
         <v>68</v>
       </c>
       <c r="M18" s="14">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="N18" s="14">
         <v>0</v>
       </c>
       <c r="O18" s="14">
+        <v>0</v>
+      </c>
+      <c r="P18" s="14">
         <v>68</v>
       </c>
-      <c r="P18" s="14">
+      <c r="Q18" s="14">
         <v>70</v>
       </c>
-      <c r="Q18" s="14">
+      <c r="R18" s="14">
         <v>55</v>
       </c>
-      <c r="R18" s="14">
+      <c r="S18" s="14">
         <v>25</v>
       </c>
-      <c r="S18" s="14">
-        <v>0</v>
-      </c>
       <c r="T18" s="14">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="U18" s="14">
         <v>60</v>
@@ -2636,8 +2703,11 @@
       <c r="W18" s="14">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X18" s="14">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>64</v>
       </c>
@@ -2672,29 +2742,29 @@
         <v>0</v>
       </c>
       <c r="L19" s="14">
+        <v>0</v>
+      </c>
+      <c r="M19" s="14">
         <v>75</v>
       </c>
-      <c r="M19" s="14">
-        <v>0</v>
-      </c>
       <c r="N19" s="14">
         <v>0</v>
       </c>
       <c r="O19" s="14">
+        <v>0</v>
+      </c>
+      <c r="P19" s="14">
         <v>75</v>
       </c>
-      <c r="P19" s="14">
-        <v>0</v>
-      </c>
       <c r="Q19" s="14">
         <v>0</v>
       </c>
       <c r="R19" s="14">
+        <v>0</v>
+      </c>
+      <c r="S19" s="14">
         <v>25</v>
       </c>
-      <c r="S19" s="14">
-        <v>0</v>
-      </c>
       <c r="T19" s="14">
         <v>0</v>
       </c>
@@ -2705,10 +2775,13 @@
         <v>0</v>
       </c>
       <c r="W19" s="14">
+        <v>0</v>
+      </c>
+      <c r="X19" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>66</v>
       </c>
@@ -2743,22 +2816,22 @@
         <v>0</v>
       </c>
       <c r="L20" s="14">
+        <v>0</v>
+      </c>
+      <c r="M20" s="14">
         <v>70</v>
       </c>
-      <c r="M20" s="14">
-        <v>0</v>
-      </c>
       <c r="N20" s="14">
         <v>0</v>
       </c>
       <c r="O20" s="14">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="P20" s="14">
         <v>70</v>
       </c>
       <c r="Q20" s="14">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="R20" s="14">
         <v>0</v>
@@ -2776,10 +2849,13 @@
         <v>0</v>
       </c>
       <c r="W20" s="14">
+        <v>0</v>
+      </c>
+      <c r="X20" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>68</v>
       </c>
@@ -2814,43 +2890,46 @@
         <v>0</v>
       </c>
       <c r="L21" s="14">
+        <v>0</v>
+      </c>
+      <c r="M21" s="14">
         <v>72</v>
       </c>
-      <c r="M21" s="14">
-        <v>0</v>
-      </c>
       <c r="N21" s="14">
         <v>0</v>
       </c>
       <c r="O21" s="14">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="P21" s="14">
         <v>72</v>
       </c>
       <c r="Q21" s="14">
+        <v>72</v>
+      </c>
+      <c r="R21" s="14">
         <v>60</v>
       </c>
-      <c r="R21" s="14">
+      <c r="S21" s="14">
         <v>25</v>
       </c>
-      <c r="S21" s="14">
-        <v>0</v>
-      </c>
       <c r="T21" s="14">
         <v>0</v>
       </c>
       <c r="U21" s="14">
+        <v>0</v>
+      </c>
+      <c r="V21" s="14">
         <v>60</v>
       </c>
-      <c r="V21" s="14">
-        <v>0</v>
-      </c>
       <c r="W21" s="14">
+        <v>0</v>
+      </c>
+      <c r="X21" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>70</v>
       </c>
@@ -2885,11 +2964,11 @@
         <v>0</v>
       </c>
       <c r="L22" s="14">
+        <v>0</v>
+      </c>
+      <c r="M22" s="14">
         <v>75</v>
       </c>
-      <c r="M22" s="14">
-        <v>0</v>
-      </c>
       <c r="N22" s="14">
         <v>0</v>
       </c>
@@ -2897,17 +2976,17 @@
         <v>0</v>
       </c>
       <c r="P22" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="14">
         <v>75</v>
       </c>
-      <c r="Q22" s="14">
-        <v>0</v>
-      </c>
       <c r="R22" s="14">
+        <v>0</v>
+      </c>
+      <c r="S22" s="14">
         <v>25</v>
       </c>
-      <c r="S22" s="14">
-        <v>0</v>
-      </c>
       <c r="T22" s="14">
         <v>0</v>
       </c>
@@ -2918,10 +2997,13 @@
         <v>0</v>
       </c>
       <c r="W22" s="14">
+        <v>0</v>
+      </c>
+      <c r="X22" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>72</v>
       </c>
@@ -2956,23 +3038,23 @@
         <v>0</v>
       </c>
       <c r="L23" s="14">
+        <v>0</v>
+      </c>
+      <c r="M23" s="14">
         <v>73</v>
       </c>
-      <c r="M23" s="14">
-        <v>0</v>
-      </c>
       <c r="N23" s="14">
         <v>0</v>
       </c>
       <c r="O23" s="14">
+        <v>0</v>
+      </c>
+      <c r="P23" s="14">
         <v>70</v>
       </c>
-      <c r="P23" s="14">
+      <c r="Q23" s="14">
         <v>73</v>
       </c>
-      <c r="Q23" s="14">
-        <v>0</v>
-      </c>
       <c r="R23" s="14">
         <v>0</v>
       </c>
@@ -2989,10 +3071,13 @@
         <v>0</v>
       </c>
       <c r="W23" s="14">
+        <v>0</v>
+      </c>
+      <c r="X23" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>74</v>
       </c>
@@ -3027,22 +3112,22 @@
         <v>71</v>
       </c>
       <c r="L24" s="14">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="M24" s="14">
         <v>71</v>
       </c>
       <c r="N24" s="14">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="O24" s="14">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="P24" s="14">
         <v>67</v>
       </c>
       <c r="Q24" s="14">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="R24" s="14">
         <v>0</v>
@@ -3062,8 +3147,11 @@
       <c r="W24" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X24" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" s="9" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>76</v>
       </c>
@@ -3133,8 +3221,11 @@
       <c r="W25" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X25" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>78</v>
       </c>
@@ -3204,8 +3295,11 @@
       <c r="W26" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X26" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>80</v>
       </c>
@@ -3240,29 +3334,29 @@
         <v>0</v>
       </c>
       <c r="L27" s="14">
+        <v>0</v>
+      </c>
+      <c r="M27" s="14">
         <v>50</v>
       </c>
-      <c r="M27" s="14">
-        <v>0</v>
-      </c>
       <c r="N27" s="14">
         <v>0</v>
       </c>
       <c r="O27" s="14">
+        <v>0</v>
+      </c>
+      <c r="P27" s="14">
         <v>43</v>
       </c>
-      <c r="P27" s="14">
+      <c r="Q27" s="14">
         <v>45</v>
       </c>
-      <c r="Q27" s="14">
-        <v>0</v>
-      </c>
       <c r="R27" s="14">
+        <v>0</v>
+      </c>
+      <c r="S27" s="14">
         <v>25</v>
       </c>
-      <c r="S27" s="14">
-        <v>0</v>
-      </c>
       <c r="T27" s="14">
         <v>0</v>
       </c>
@@ -3275,8 +3369,11 @@
       <c r="W27" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X27" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>82</v>
       </c>
@@ -3311,23 +3408,23 @@
         <v>0</v>
       </c>
       <c r="L28" s="14">
+        <v>0</v>
+      </c>
+      <c r="M28" s="14">
         <v>50</v>
       </c>
-      <c r="M28" s="14">
-        <v>0</v>
-      </c>
       <c r="N28" s="14">
         <v>0</v>
       </c>
       <c r="O28" s="14">
+        <v>0</v>
+      </c>
+      <c r="P28" s="14">
         <v>43</v>
       </c>
-      <c r="P28" s="14">
+      <c r="Q28" s="14">
         <v>48</v>
       </c>
-      <c r="Q28" s="14">
-        <v>0</v>
-      </c>
       <c r="R28" s="14">
         <v>0</v>
       </c>
@@ -3346,8 +3443,11 @@
       <c r="W28" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X28" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>84</v>
       </c>
@@ -3391,11 +3491,11 @@
         <v>0</v>
       </c>
       <c r="O29" s="14">
+        <v>0</v>
+      </c>
+      <c r="P29" s="14">
         <v>70</v>
       </c>
-      <c r="P29" s="14">
-        <v>0</v>
-      </c>
       <c r="Q29" s="14">
         <v>0</v>
       </c>
@@ -3417,8 +3517,11 @@
       <c r="W29" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X29" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>86</v>
       </c>
@@ -3488,8 +3591,11 @@
       <c r="W30" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X30" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>88</v>
       </c>
@@ -3524,29 +3630,29 @@
         <v>0</v>
       </c>
       <c r="L31" s="14">
+        <v>0</v>
+      </c>
+      <c r="M31" s="14">
         <v>73</v>
       </c>
-      <c r="M31" s="14">
-        <v>0</v>
-      </c>
       <c r="N31" s="14">
         <v>0</v>
       </c>
       <c r="O31" s="14">
+        <v>0</v>
+      </c>
+      <c r="P31" s="14">
         <v>70</v>
       </c>
-      <c r="P31" s="14">
+      <c r="Q31" s="14">
         <v>73</v>
       </c>
-      <c r="Q31" s="14">
-        <v>0</v>
-      </c>
       <c r="R31" s="14">
+        <v>0</v>
+      </c>
+      <c r="S31" s="14">
         <v>25</v>
       </c>
-      <c r="S31" s="14">
-        <v>0</v>
-      </c>
       <c r="T31" s="14">
         <v>0</v>
       </c>
@@ -3557,10 +3663,13 @@
         <v>0</v>
       </c>
       <c r="W31" s="14">
+        <v>0</v>
+      </c>
+      <c r="X31" s="14">
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>90</v>
       </c>
@@ -3595,22 +3704,22 @@
         <v>0</v>
       </c>
       <c r="L32" s="14">
+        <v>0</v>
+      </c>
+      <c r="M32" s="14">
         <v>49</v>
       </c>
-      <c r="M32" s="14">
-        <v>0</v>
-      </c>
       <c r="N32" s="14">
         <v>0</v>
       </c>
       <c r="O32" s="14">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="P32" s="14">
         <v>47</v>
       </c>
       <c r="Q32" s="14">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="R32" s="14">
         <v>0</v>
@@ -3630,8 +3739,11 @@
       <c r="W32" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X32" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>92</v>
       </c>
@@ -3666,22 +3778,22 @@
         <v>0</v>
       </c>
       <c r="L33" s="14">
+        <v>0</v>
+      </c>
+      <c r="M33" s="14">
         <v>123</v>
       </c>
-      <c r="M33" s="14">
-        <v>0</v>
-      </c>
       <c r="N33" s="14">
         <v>0</v>
       </c>
       <c r="O33" s="14">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="P33" s="14">
         <v>120</v>
       </c>
       <c r="Q33" s="14">
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="R33" s="14">
         <v>0</v>
@@ -3701,8 +3813,11 @@
       <c r="W33" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X33" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>94</v>
       </c>
@@ -3737,23 +3852,23 @@
         <v>0</v>
       </c>
       <c r="L34" s="14">
+        <v>0</v>
+      </c>
+      <c r="M34" s="14">
         <v>50</v>
       </c>
-      <c r="M34" s="14">
-        <v>0</v>
-      </c>
       <c r="N34" s="14">
         <v>0</v>
       </c>
       <c r="O34" s="14">
+        <v>0</v>
+      </c>
+      <c r="P34" s="14">
         <v>44</v>
       </c>
-      <c r="P34" s="14">
+      <c r="Q34" s="14">
         <v>48</v>
       </c>
-      <c r="Q34" s="14">
-        <v>0</v>
-      </c>
       <c r="R34" s="14">
         <v>0</v>
       </c>
@@ -3772,8 +3887,11 @@
       <c r="W34" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X34" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>96</v>
       </c>
@@ -3808,22 +3926,22 @@
         <v>0</v>
       </c>
       <c r="L35" s="14">
+        <v>0</v>
+      </c>
+      <c r="M35" s="14">
         <v>50</v>
       </c>
-      <c r="M35" s="14">
-        <v>0</v>
-      </c>
       <c r="N35" s="14">
         <v>0</v>
       </c>
       <c r="O35" s="14">
-        <v>75</v>
+        <v>0</v>
       </c>
       <c r="P35" s="14">
         <v>75</v>
       </c>
       <c r="Q35" s="14">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="R35" s="14">
         <v>0</v>
@@ -3843,8 +3961,11 @@
       <c r="W35" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X35" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>98</v>
       </c>
@@ -3914,8 +4035,11 @@
       <c r="W36" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X36" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>100</v>
       </c>
@@ -3950,11 +4074,11 @@
         <v>0</v>
       </c>
       <c r="L37" s="14">
+        <v>0</v>
+      </c>
+      <c r="M37" s="14">
         <v>135</v>
       </c>
-      <c r="M37" s="14">
-        <v>0</v>
-      </c>
       <c r="N37" s="14">
         <v>0</v>
       </c>
@@ -3965,28 +4089,31 @@
         <v>0</v>
       </c>
       <c r="Q37" s="14">
+        <v>0</v>
+      </c>
+      <c r="R37" s="14">
         <v>123</v>
       </c>
-      <c r="R37" s="14">
+      <c r="S37" s="14">
         <v>85</v>
       </c>
-      <c r="S37" s="14">
-        <v>0</v>
-      </c>
       <c r="T37" s="14">
         <v>0</v>
       </c>
       <c r="U37" s="14">
+        <v>0</v>
+      </c>
+      <c r="V37" s="14">
         <v>114</v>
       </c>
-      <c r="V37" s="14">
-        <v>0</v>
-      </c>
       <c r="W37" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X37" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>102</v>
       </c>
@@ -4030,20 +4157,20 @@
         <v>0</v>
       </c>
       <c r="O38" s="14">
+        <v>0</v>
+      </c>
+      <c r="P38" s="14">
         <v>75</v>
       </c>
-      <c r="P38" s="14">
-        <v>0</v>
-      </c>
       <c r="Q38" s="14">
         <v>0</v>
       </c>
       <c r="R38" s="14">
+        <v>0</v>
+      </c>
+      <c r="S38" s="14">
         <v>25</v>
       </c>
-      <c r="S38" s="14">
-        <v>0</v>
-      </c>
       <c r="T38" s="14">
         <v>0</v>
       </c>
@@ -4056,8 +4183,11 @@
       <c r="W38" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X38" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>104</v>
       </c>
@@ -4125,10 +4255,13 @@
         <v>0</v>
       </c>
       <c r="W39" s="14">
+        <v>0</v>
+      </c>
+      <c r="X39" s="14">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>106</v>
       </c>
@@ -4172,11 +4305,11 @@
         <v>0</v>
       </c>
       <c r="O40" s="14">
+        <v>0</v>
+      </c>
+      <c r="P40" s="14">
         <v>75</v>
       </c>
-      <c r="P40" s="14">
-        <v>0</v>
-      </c>
       <c r="Q40" s="14">
         <v>0</v>
       </c>
@@ -4190,16 +4323,19 @@
         <v>0</v>
       </c>
       <c r="U40" s="14">
+        <v>0</v>
+      </c>
+      <c r="V40" s="14">
         <v>60</v>
       </c>
-      <c r="V40" s="14">
-        <v>0</v>
-      </c>
       <c r="W40" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X40" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>108</v>
       </c>
@@ -4249,11 +4385,11 @@
         <v>0</v>
       </c>
       <c r="Q41" s="14">
+        <v>0</v>
+      </c>
+      <c r="R41" s="14">
         <v>50</v>
       </c>
-      <c r="R41" s="14">
-        <v>0</v>
-      </c>
       <c r="S41" s="14">
         <v>0</v>
       </c>
@@ -4269,8 +4405,11 @@
       <c r="W41" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X41" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>110</v>
       </c>
@@ -4332,16 +4471,19 @@
         <v>0</v>
       </c>
       <c r="U42" s="14">
+        <v>0</v>
+      </c>
+      <c r="V42" s="14">
         <v>60</v>
       </c>
-      <c r="V42" s="14">
-        <v>0</v>
-      </c>
       <c r="W42" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X42" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>112</v>
       </c>
@@ -4376,20 +4518,20 @@
         <v>0</v>
       </c>
       <c r="L43" s="14">
+        <v>0</v>
+      </c>
+      <c r="M43" s="14">
         <v>110</v>
       </c>
-      <c r="M43" s="14">
-        <v>0</v>
-      </c>
       <c r="N43" s="14">
         <v>0</v>
       </c>
       <c r="O43" s="14">
+        <v>0</v>
+      </c>
+      <c r="P43" s="14">
         <v>110</v>
       </c>
-      <c r="P43" s="14">
-        <v>0</v>
-      </c>
       <c r="Q43" s="14">
         <v>0</v>
       </c>
@@ -4403,16 +4545,19 @@
         <v>0</v>
       </c>
       <c r="U43" s="14">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="V43" s="14">
         <v>95</v>
       </c>
       <c r="W43" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>95</v>
+      </c>
+      <c r="X43" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>114</v>
       </c>
@@ -4462,14 +4607,14 @@
         <v>0</v>
       </c>
       <c r="Q44" s="14">
+        <v>0</v>
+      </c>
+      <c r="R44" s="14">
         <v>10</v>
       </c>
-      <c r="R44" s="14">
+      <c r="S44" s="14">
         <v>16</v>
       </c>
-      <c r="S44" s="14">
-        <v>0</v>
-      </c>
       <c r="T44" s="14">
         <v>0</v>
       </c>
@@ -4480,10 +4625,13 @@
         <v>0</v>
       </c>
       <c r="W44" s="14">
+        <v>0</v>
+      </c>
+      <c r="X44" s="14">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>116</v>
       </c>
@@ -4518,23 +4666,23 @@
         <v>0</v>
       </c>
       <c r="L45" s="14">
+        <v>0</v>
+      </c>
+      <c r="M45" s="14">
         <v>75</v>
       </c>
-      <c r="M45" s="14">
-        <v>0</v>
-      </c>
       <c r="N45" s="14">
         <v>0</v>
       </c>
       <c r="O45" s="14">
+        <v>0</v>
+      </c>
+      <c r="P45" s="14">
         <v>70</v>
       </c>
-      <c r="P45" s="14">
+      <c r="Q45" s="14">
         <v>75</v>
       </c>
-      <c r="Q45" s="14">
-        <v>0</v>
-      </c>
       <c r="R45" s="14">
         <v>0</v>
       </c>
@@ -4553,8 +4701,11 @@
       <c r="W45" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X45" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>118</v>
       </c>
@@ -4589,28 +4740,28 @@
         <v>0</v>
       </c>
       <c r="L46" s="14">
+        <v>0</v>
+      </c>
+      <c r="M46" s="14">
         <v>103</v>
       </c>
-      <c r="M46" s="14">
-        <v>0</v>
-      </c>
       <c r="N46" s="14">
         <v>0</v>
       </c>
       <c r="O46" s="14">
+        <v>0</v>
+      </c>
+      <c r="P46" s="14">
         <v>98</v>
       </c>
-      <c r="P46" s="14">
-        <v>0</v>
-      </c>
       <c r="Q46" s="14">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="R46" s="14">
         <v>25</v>
       </c>
       <c r="S46" s="14">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="T46" s="14">
         <v>0</v>
@@ -4624,8 +4775,11 @@
       <c r="W46" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X46" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>119</v>
       </c>
@@ -4660,43 +4814,46 @@
         <v>0</v>
       </c>
       <c r="L47" s="14">
+        <v>0</v>
+      </c>
+      <c r="M47" s="14">
         <v>75</v>
       </c>
-      <c r="M47" s="14">
-        <v>0</v>
-      </c>
       <c r="N47" s="14">
         <v>0</v>
       </c>
       <c r="O47" s="14">
+        <v>0</v>
+      </c>
+      <c r="P47" s="14">
         <v>75</v>
       </c>
-      <c r="P47" s="14">
-        <v>0</v>
-      </c>
       <c r="Q47" s="14">
         <v>0</v>
       </c>
       <c r="R47" s="14">
+        <v>0</v>
+      </c>
+      <c r="S47" s="14">
         <v>25</v>
       </c>
-      <c r="S47" s="14">
-        <v>0</v>
-      </c>
       <c r="T47" s="14">
         <v>0</v>
       </c>
       <c r="U47" s="14">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="V47" s="14">
         <v>50</v>
       </c>
       <c r="W47" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="X47" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:24" s="9" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>121</v>
       </c>
@@ -4749,11 +4906,11 @@
         <v>0</v>
       </c>
       <c r="R48" s="14">
+        <v>0</v>
+      </c>
+      <c r="S48" s="14">
         <v>25</v>
       </c>
-      <c r="S48" s="14">
-        <v>0</v>
-      </c>
       <c r="T48" s="14">
         <v>0</v>
       </c>
@@ -4766,8 +4923,11 @@
       <c r="W48" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X48" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>123</v>
       </c>
@@ -4820,11 +4980,11 @@
         <v>0</v>
       </c>
       <c r="R49" s="14">
+        <v>0</v>
+      </c>
+      <c r="S49" s="14">
         <v>25</v>
       </c>
-      <c r="S49" s="14">
-        <v>0</v>
-      </c>
       <c r="T49" s="14">
         <v>0</v>
       </c>
@@ -4837,8 +4997,11 @@
       <c r="W49" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X49" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>125</v>
       </c>
@@ -4873,23 +5036,23 @@
         <v>88</v>
       </c>
       <c r="L50" s="14">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="M50" s="14">
         <v>88</v>
       </c>
       <c r="N50" s="14">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="O50" s="14">
         <v>0</v>
       </c>
       <c r="P50" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="14">
         <v>88</v>
       </c>
-      <c r="Q50" s="14">
-        <v>0</v>
-      </c>
       <c r="R50" s="14">
         <v>0</v>
       </c>
@@ -4908,8 +5071,11 @@
       <c r="W50" s="14">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X50" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>127</v>
       </c>
@@ -4944,16 +5110,16 @@
         <v>0</v>
       </c>
       <c r="L51" s="14">
+        <v>0</v>
+      </c>
+      <c r="M51" s="14">
         <v>80</v>
       </c>
-      <c r="M51" s="14">
-        <v>0</v>
-      </c>
       <c r="N51" s="14">
         <v>0</v>
       </c>
       <c r="O51" s="14">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="P51" s="14">
         <v>70</v>
@@ -4962,13 +5128,13 @@
         <v>70</v>
       </c>
       <c r="R51" s="14">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="S51" s="14">
         <v>25</v>
       </c>
       <c r="T51" s="14">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="U51" s="14">
         <v>0</v>
@@ -4977,10 +5143,13 @@
         <v>0</v>
       </c>
       <c r="W51" s="14">
+        <v>0</v>
+      </c>
+      <c r="X51" s="14">
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>163</v>
       </c>
@@ -5015,13 +5184,13 @@
         <v>0</v>
       </c>
       <c r="L52" s="14">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="M52" s="14">
         <v>70</v>
       </c>
       <c r="N52" s="14">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="O52" s="14">
         <v>0</v>
@@ -5033,13 +5202,13 @@
         <v>0</v>
       </c>
       <c r="R52" s="14">
+        <v>0</v>
+      </c>
+      <c r="S52" s="14">
         <v>25</v>
       </c>
-      <c r="S52" s="14">
-        <v>0</v>
-      </c>
       <c r="T52" s="14">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="U52" s="14">
         <v>55</v>
@@ -5050,8 +5219,11 @@
       <c r="W52" s="14">
         <v>55</v>
       </c>
-    </row>
-    <row r="53" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="X52" s="14">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="53" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>165</v>
       </c>
@@ -5086,16 +5258,16 @@
         <v>0</v>
       </c>
       <c r="L53" s="14">
+        <v>0</v>
+      </c>
+      <c r="M53" s="14">
         <v>80</v>
       </c>
-      <c r="M53" s="14">
-        <v>0</v>
-      </c>
       <c r="N53" s="14">
         <v>0</v>
       </c>
       <c r="O53" s="14">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="P53" s="14">
         <v>70</v>
@@ -5104,13 +5276,13 @@
         <v>70</v>
       </c>
       <c r="R53" s="14">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="S53" s="14">
         <v>25</v>
       </c>
       <c r="T53" s="14">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="U53" s="14">
         <v>0</v>
@@ -5119,6 +5291,9 @@
         <v>0</v>
       </c>
       <c r="W53" s="14">
+        <v>0</v>
+      </c>
+      <c r="X53" s="14">
         <v>60</v>
       </c>
     </row>
@@ -5131,10 +5306,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5176,123 +5351,139 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
         <v>133</v>
       </c>
       <c r="C5" s="24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+    <row r="7" spans="2:3" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="23" t="s">
         <v>133</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C7" s="24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="21" t="s">
+    <row r="9" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C9" s="24" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="21" t="s">
-        <v>135</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="23" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C11" s="22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="21" t="s">
+    <row r="13" spans="2:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C13" s="22" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C16" s="22" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="21" t="s">
+    <row r="17" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
         <v>139</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C17" s="22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="23" t="s">
+    <row r="18" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="23" t="s">
         <v>140</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C18" s="24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="23" t="s">
+    <row r="19" spans="2:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C19" s="24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="23" t="s">
+    <row r="20" spans="2:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C20" s="24" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="2:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="25" t="s">
+    <row r="21" spans="2:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C21" s="26" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>